<commit_message>
Better Analysis, still going. Also UI updates to MCAO Lookup
</commit_message>
<xml_diff>
--- a/apps/gsrealty-client/gsrealty-client-template.xlsx
+++ b/apps/gsrealty-client/gsrealty-client-template.xlsx
@@ -1,27 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrettsullivan/Desktop/‼️/RE/RealtyONE/MY LISTINGS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrettsullivan/Desktop/AUTOMATE/Vibe Code/Wabbit/clients/sullivan_realestate/Actual/apps/gsrealty-client/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81B00CF1-FB79-9D49-9ADE-C5A2880D3D56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B97D1CFB-13BF-EC4D-B5BF-19A3EF892957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15960" windowHeight="22400" activeTab="3" xr2:uid="{8428AA42-3A5B-9D4D-91E2-2CA67F06E6B1}"/>
+    <workbookView xWindow="1000" yWindow="10620" windowWidth="31240" windowHeight="11780" activeTab="3" xr2:uid="{8428AA42-3A5B-9D4D-91E2-2CA67F06E6B1}"/>
   </bookViews>
   <sheets>
-    <sheet name="comps" sheetId="7" r:id="rId1"/>
-    <sheet name="Full_API_call" sheetId="6" r:id="rId2"/>
-    <sheet name="Analysis" sheetId="8" r:id="rId3"/>
-    <sheet name="Calcs" sheetId="3" r:id="rId4"/>
-    <sheet name="Maricopa" sheetId="1" r:id="rId5"/>
-    <sheet name=".5mile" sheetId="11" r:id="rId6"/>
-    <sheet name="Lot" sheetId="2" r:id="rId7"/>
+    <sheet name="MLS-Resi-Comps" sheetId="7" r:id="rId1"/>
+    <sheet name="MLS-Lease-Comps" sheetId="9" r:id="rId2"/>
+    <sheet name="Full-MCAO-API" sheetId="6" r:id="rId3"/>
+    <sheet name="Analysis" sheetId="8" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,104 +39,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="418">
-  <si>
-    <t>Owner Information</t>
-  </si>
-  <si>
-    <t>Owner Name:</t>
-  </si>
-  <si>
-    <t>In Care Of:</t>
-  </si>
-  <si>
-    <t>Property Address:</t>
-  </si>
-  <si>
-    <t>Mailing Address:</t>
-  </si>
-  <si>
-    <t>Deed Number:</t>
-  </si>
-  <si>
-    <t>Sale Date:</t>
-  </si>
-  <si>
-    <t>Sale Price:</t>
-  </si>
-  <si>
-    <t>Property Information</t>
-  </si>
-  <si>
-    <t>Lat/Long:</t>
-  </si>
-  <si>
-    <t>S/T/R:</t>
-  </si>
-  <si>
-    <t>Jurisdiction:</t>
-  </si>
-  <si>
-    <t>PUC:</t>
-  </si>
-  <si>
-    <t>Lot Size (sq ft):</t>
-  </si>
-  <si>
-    <t>MCR #:</t>
-  </si>
-  <si>
-    <t>Subdivision:</t>
-  </si>
-  <si>
-    <t>Lot #:</t>
-  </si>
-  <si>
-    <t>Tract/Block:</t>
-  </si>
-  <si>
-    <t>Floor:</t>
-  </si>
-  <si>
-    <t>Construction Year:</t>
-  </si>
-  <si>
-    <t>Living Space (sq ft):</t>
-  </si>
-  <si>
-    <t>Valuation Information</t>
-  </si>
-  <si>
-    <t>Tax Year:</t>
-  </si>
-  <si>
-    <t>2026 </t>
-  </si>
-  <si>
-    <t>2025 </t>
-  </si>
-  <si>
-    <t>FCV:</t>
-  </si>
-  <si>
-    <t>LPV:</t>
-  </si>
-  <si>
-    <t>Legal Class:</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="428">
   <si>
     <t>APN</t>
   </si>
   <si>
-    <t>Basis</t>
-  </si>
-  <si>
-    <t>Basis Date</t>
-  </si>
-  <si>
-    <t>Maricopa Tax valuation</t>
-  </si>
-  <si>
     <t>MCR</t>
   </si>
   <si>
@@ -1292,72 +1196,143 @@
     <t>Features</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
     <t>Item</t>
+  </si>
+  <si>
+    <t>BR</t>
+  </si>
+  <si>
+    <t>BA</t>
+  </si>
+  <si>
+    <t>SQFT</t>
+  </si>
+  <si>
+    <t>STATUS</t>
+  </si>
+  <si>
+    <t>SALE_PRICE</t>
+  </si>
+  <si>
+    <t>OG_LIST_PRICE</t>
+  </si>
+  <si>
+    <t>OG_LIST_DATE</t>
+  </si>
+  <si>
+    <t>SALE_DATE</t>
+  </si>
+  <si>
+    <t>SELLER_BASIS</t>
+  </si>
+  <si>
+    <t>SELLER_BASIS_DATE</t>
+  </si>
+  <si>
+    <t>ITEM</t>
+  </si>
+  <si>
+    <t>LOT_SIZE</t>
+  </si>
+  <si>
+    <t>MLS_MCAO_DISCREPENCY_CONCAT</t>
+  </si>
+  <si>
+    <t>FULL_ADDRESS</t>
+  </si>
+  <si>
+    <t>IS_RENTAL</t>
+  </si>
+  <si>
+    <t>RENOVATE_SCORE</t>
+  </si>
+  <si>
+    <t>LINK</t>
+  </si>
+  <si>
+    <t>IN_MLS?</t>
+  </si>
+  <si>
+    <t>IN_MCAO?</t>
+  </si>
+  <si>
+    <t>CANCEL_DATE</t>
+  </si>
+  <si>
+    <t>UC_DATE</t>
+  </si>
+  <si>
+    <t>LAT</t>
+  </si>
+  <si>
+    <t>LON</t>
+  </si>
+  <si>
+    <t>YEAR_BUILT</t>
+  </si>
+  <si>
+    <t>DAYS_ON_MARKET</t>
+  </si>
+  <si>
+    <t>DWELLING_TYPE</t>
+  </si>
+  <si>
+    <t>SUBDIVISION_NAME</t>
+  </si>
+  <si>
+    <t>PROPERTY_RADAR-COMP-Y-N</t>
+  </si>
+  <si>
+    <t>Item (Residential 1.5 Mile Comps, Residential Lease 1.5 Mile Comps, Residential 3 yr Direct Subdivision Comps, Residential Leaase 3yr Direct Subdivision Comps)</t>
+  </si>
+  <si>
+    <t>Lease Start Date</t>
+  </si>
+  <si>
+    <t>Lease Sign Date</t>
+  </si>
+  <si>
+    <t>UCB</t>
+  </si>
+  <si>
+    <t>Lease Price/HiSeason</t>
+  </si>
+  <si>
+    <t>Mthly Rate Hi Season</t>
+  </si>
+  <si>
+    <t>Mthly Rate Lo Season</t>
+  </si>
+  <si>
+    <t>Price Per SqFt</t>
+  </si>
+  <si>
+    <t>Sold Price Per SqFt</t>
+  </si>
+  <si>
+    <t>Owner Name - DND2</t>
+  </si>
+  <si>
+    <t>Vacation Ready Rental Y/N</t>
+  </si>
+  <si>
+    <t>Date Available</t>
+  </si>
+  <si>
+    <t>Booking Availability End Date</t>
+  </si>
+  <si>
+    <t>Rental Beast Apply Now</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF132048"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1391,6 +1366,31 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1401,7 +1401,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1430,41 +1430,39 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="4" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
-    <cellStyle name="Currency" xfId="1" builtinId="4"/>
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
-    <cellStyle name="Hyperlink 2" xfId="4" xr:uid="{7471C002-520F-1444-9836-6A76B16417A3}"/>
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink 2" xfId="2" xr:uid="{7471C002-520F-1444-9836-6A76B16417A3}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3" xr:uid="{41B3FAE6-1A06-4940-82B5-3FBBE542BF08}"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{41B3FAE6-1A06-4940-82B5-3FBBE542BF08}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1477,55 +1475,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>292100</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>76199</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>660400</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>48520</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3652EFF-0F81-F140-80EF-A1BF35DBBD58}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="292100" y="76199"/>
-          <a:ext cx="4495800" cy="6474721"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1847,8 +1796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C275542-9725-164C-86E3-957028673AA5}">
   <dimension ref="A1:CV48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="BR1" workbookViewId="0">
+      <selection activeCell="CC1" sqref="CC1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1856,628 +1805,618 @@
     <col min="1" max="1" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:100" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
-        <v>416</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:100" s="9" customFormat="1" ht="58" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>385</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>294</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>296</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="Q1" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="R1" s="9" t="s">
+        <v>302</v>
+      </c>
+      <c r="S1" s="9" t="s">
+        <v>303</v>
+      </c>
+      <c r="T1" s="9" t="s">
+        <v>304</v>
+      </c>
+      <c r="U1" s="9" t="s">
+        <v>305</v>
+      </c>
+      <c r="V1" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="W1" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="X1" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="Y1" s="9" t="s">
+        <v>309</v>
+      </c>
+      <c r="Z1" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="AA1" s="9" t="s">
+        <v>311</v>
+      </c>
+      <c r="AB1" s="9" t="s">
+        <v>312</v>
+      </c>
+      <c r="AC1" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="AD1" s="9" t="s">
+        <v>314</v>
+      </c>
+      <c r="AE1" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="AF1" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="AG1" s="9" t="s">
         <v>317</v>
       </c>
-      <c r="C1" t="s">
+      <c r="AH1" s="9" t="s">
         <v>318</v>
       </c>
-      <c r="D1" t="s">
+      <c r="AI1" s="9" t="s">
         <v>319</v>
       </c>
-      <c r="E1" t="s">
+      <c r="AJ1" s="9" t="s">
         <v>320</v>
       </c>
-      <c r="F1" t="s">
+      <c r="AK1" s="9" t="s">
         <v>321</v>
       </c>
-      <c r="G1" t="s">
+      <c r="AL1" s="9" t="s">
         <v>322</v>
       </c>
-      <c r="H1" t="s">
+      <c r="AM1" s="9" t="s">
         <v>323</v>
       </c>
-      <c r="I1" t="s">
+      <c r="AN1" s="9" t="s">
         <v>324</v>
       </c>
-      <c r="J1" t="s">
+      <c r="AO1" s="9" t="s">
         <v>325</v>
       </c>
-      <c r="K1" t="s">
+      <c r="AP1" s="9" t="s">
         <v>326</v>
       </c>
-      <c r="L1" t="s">
+      <c r="AQ1" s="9" t="s">
         <v>327</v>
       </c>
-      <c r="M1" t="s">
+      <c r="AR1" s="9" t="s">
         <v>328</v>
       </c>
-      <c r="N1" t="s">
+      <c r="AS1" s="9" t="s">
         <v>329</v>
       </c>
-      <c r="O1" t="s">
+      <c r="AT1" s="9" t="s">
         <v>330</v>
       </c>
-      <c r="P1" t="s">
+      <c r="AU1" s="9" t="s">
         <v>331</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="AV1" s="9" t="s">
         <v>332</v>
       </c>
-      <c r="R1" t="s">
+      <c r="AW1" s="9" t="s">
         <v>333</v>
       </c>
-      <c r="S1" t="s">
+      <c r="AX1" s="9" t="s">
         <v>334</v>
       </c>
-      <c r="T1" t="s">
+      <c r="AY1" s="9" t="s">
         <v>335</v>
       </c>
-      <c r="U1" t="s">
+      <c r="AZ1" s="9" t="s">
         <v>336</v>
       </c>
-      <c r="V1" t="s">
+      <c r="BA1" s="9" t="s">
         <v>337</v>
       </c>
-      <c r="W1" t="s">
+      <c r="BB1" s="9" t="s">
         <v>338</v>
       </c>
-      <c r="X1" t="s">
+      <c r="BC1" s="9" t="s">
         <v>339</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="BD1" s="9" t="s">
         <v>340</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="BE1" s="9" t="s">
         <v>341</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="BF1" s="9" t="s">
         <v>342</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="BG1" s="9" t="s">
         <v>343</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="BH1" s="9" t="s">
         <v>344</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="BI1" s="9" t="s">
         <v>345</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="BJ1" s="9" t="s">
         <v>346</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="BK1" s="9" t="s">
         <v>347</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="BL1" s="9" t="s">
         <v>348</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="BM1" s="9" t="s">
         <v>349</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="BN1" s="9" t="s">
         <v>350</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="BO1" s="9" t="s">
         <v>351</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="BP1" s="9" t="s">
         <v>352</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="BQ1" s="9" t="s">
         <v>353</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="BR1" s="9" t="s">
         <v>354</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="BS1" s="9" t="s">
         <v>355</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="BT1" s="9" t="s">
         <v>356</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="BU1" s="9" t="s">
         <v>357</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="BV1" s="9" t="s">
         <v>358</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="BW1" s="9" t="s">
         <v>359</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="BX1" s="9" t="s">
         <v>360</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="BY1" s="9" t="s">
         <v>361</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="BZ1" s="9" t="s">
         <v>362</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="CA1" s="9" t="s">
         <v>363</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="CB1" s="9" t="s">
         <v>364</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="CC1" s="9" t="s">
         <v>365</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="CD1" s="9" t="s">
         <v>366</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="CE1" s="9" t="s">
         <v>367</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="CF1" s="9" t="s">
         <v>368</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="CG1" s="9" t="s">
         <v>369</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="CH1" s="9" t="s">
         <v>370</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="CI1" s="9" t="s">
         <v>371</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="CJ1" s="9" t="s">
         <v>372</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="CK1" s="9" t="s">
         <v>373</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="CL1" s="9" t="s">
         <v>374</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="CM1" s="9" t="s">
         <v>375</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="CN1" s="9" t="s">
         <v>376</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="CO1" s="9" t="s">
         <v>377</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="CP1" s="9" t="s">
         <v>378</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="CQ1" s="9" t="s">
         <v>379</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="CR1" s="9" t="s">
         <v>380</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="CS1" s="9" t="s">
         <v>381</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="CT1" s="9" t="s">
         <v>382</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="CU1" s="9" t="s">
         <v>383</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="CV1" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="BR1" t="s">
-        <v>385</v>
-      </c>
-      <c r="BS1" t="s">
-        <v>386</v>
-      </c>
-      <c r="BT1" t="s">
-        <v>387</v>
-      </c>
-      <c r="BU1" t="s">
-        <v>388</v>
-      </c>
-      <c r="BV1" t="s">
-        <v>389</v>
-      </c>
-      <c r="BW1" t="s">
-        <v>390</v>
-      </c>
-      <c r="BX1" t="s">
-        <v>391</v>
-      </c>
-      <c r="BY1" t="s">
-        <v>392</v>
-      </c>
-      <c r="BZ1" t="s">
-        <v>393</v>
-      </c>
-      <c r="CA1" t="s">
-        <v>394</v>
-      </c>
-      <c r="CB1" t="s">
-        <v>395</v>
-      </c>
-      <c r="CC1" t="s">
-        <v>396</v>
-      </c>
-      <c r="CD1" t="s">
-        <v>397</v>
-      </c>
-      <c r="CE1" t="s">
-        <v>398</v>
-      </c>
-      <c r="CF1" t="s">
-        <v>399</v>
-      </c>
-      <c r="CG1" t="s">
-        <v>400</v>
-      </c>
-      <c r="CH1" t="s">
-        <v>401</v>
-      </c>
-      <c r="CI1" t="s">
-        <v>402</v>
-      </c>
-      <c r="CJ1" t="s">
-        <v>403</v>
-      </c>
-      <c r="CK1" t="s">
-        <v>404</v>
-      </c>
-      <c r="CL1" t="s">
-        <v>405</v>
-      </c>
-      <c r="CM1" t="s">
-        <v>406</v>
-      </c>
-      <c r="CN1" t="s">
-        <v>407</v>
-      </c>
-      <c r="CO1" t="s">
-        <v>408</v>
-      </c>
-      <c r="CP1" t="s">
-        <v>409</v>
-      </c>
-      <c r="CQ1" t="s">
-        <v>410</v>
-      </c>
-      <c r="CR1" t="s">
-        <v>411</v>
-      </c>
-      <c r="CS1" t="s">
-        <v>412</v>
-      </c>
-      <c r="CT1" t="s">
-        <v>413</v>
-      </c>
-      <c r="CU1" t="s">
-        <v>414</v>
-      </c>
-      <c r="CV1" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="2" spans="1:100" x14ac:dyDescent="0.2">
-      <c r="N2" s="13"/>
-      <c r="S2" s="13"/>
-      <c r="BI2" s="14"/>
-    </row>
-    <row r="3" spans="1:100" x14ac:dyDescent="0.2">
-      <c r="N3" s="13"/>
-      <c r="S3" s="13"/>
-      <c r="BI3" s="14"/>
     </row>
     <row r="4" spans="1:100" x14ac:dyDescent="0.2">
-      <c r="N4" s="13"/>
-      <c r="S4" s="13"/>
-      <c r="BI4" s="14"/>
-      <c r="CJ4" s="13"/>
+      <c r="N4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="BI4" s="6"/>
+      <c r="CJ4" s="5"/>
     </row>
     <row r="5" spans="1:100" x14ac:dyDescent="0.2">
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-      <c r="S5" s="13"/>
-      <c r="BI5" s="14"/>
-      <c r="CD5" s="13"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="BI5" s="6"/>
+      <c r="CD5" s="5"/>
     </row>
     <row r="6" spans="1:100" x14ac:dyDescent="0.2">
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="13"/>
-      <c r="S6" s="13"/>
-      <c r="BI6" s="14"/>
-      <c r="CD6" s="13"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="BI6" s="6"/>
+      <c r="CD6" s="5"/>
     </row>
     <row r="7" spans="1:100" x14ac:dyDescent="0.2">
-      <c r="N7" s="13"/>
-      <c r="S7" s="13"/>
-      <c r="BI7" s="14"/>
-      <c r="CJ7" s="13"/>
+      <c r="N7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="BI7" s="6"/>
+      <c r="CJ7" s="5"/>
     </row>
     <row r="8" spans="1:100" x14ac:dyDescent="0.2">
-      <c r="N8" s="13"/>
-      <c r="S8" s="13"/>
-      <c r="BI8" s="14"/>
-      <c r="CJ8" s="13"/>
+      <c r="N8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="BI8" s="6"/>
+      <c r="CJ8" s="5"/>
     </row>
     <row r="9" spans="1:100" x14ac:dyDescent="0.2">
-      <c r="N9" s="13"/>
-      <c r="S9" s="13"/>
-      <c r="U9" s="13"/>
-      <c r="BI9" s="14"/>
-      <c r="CD9" s="13"/>
+      <c r="N9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="U9" s="5"/>
+      <c r="BI9" s="6"/>
+      <c r="CD9" s="5"/>
     </row>
     <row r="10" spans="1:100" x14ac:dyDescent="0.2">
-      <c r="N10" s="13"/>
-      <c r="S10" s="13"/>
-      <c r="U10" s="13"/>
-      <c r="BI10" s="14"/>
-      <c r="CD10" s="13"/>
+      <c r="N10" s="5"/>
+      <c r="S10" s="5"/>
+      <c r="U10" s="5"/>
+      <c r="BI10" s="6"/>
+      <c r="CD10" s="5"/>
     </row>
     <row r="11" spans="1:100" x14ac:dyDescent="0.2">
-      <c r="N11" s="13"/>
-      <c r="S11" s="13"/>
-      <c r="BI11" s="14"/>
-      <c r="CD11" s="13"/>
-      <c r="CJ11" s="13"/>
+      <c r="N11" s="5"/>
+      <c r="S11" s="5"/>
+      <c r="BI11" s="6"/>
+      <c r="CD11" s="5"/>
+      <c r="CJ11" s="5"/>
     </row>
     <row r="12" spans="1:100" x14ac:dyDescent="0.2">
-      <c r="N12" s="13"/>
-      <c r="S12" s="13"/>
-      <c r="BI12" s="14"/>
-      <c r="CD12" s="13"/>
-      <c r="CJ12" s="13"/>
+      <c r="N12" s="5"/>
+      <c r="S12" s="5"/>
+      <c r="BI12" s="6"/>
+      <c r="CD12" s="5"/>
+      <c r="CJ12" s="5"/>
     </row>
     <row r="13" spans="1:100" x14ac:dyDescent="0.2">
-      <c r="N13" s="13"/>
-      <c r="Q13" s="13"/>
-      <c r="S13" s="13"/>
-      <c r="T13" s="13"/>
-      <c r="BI13" s="14"/>
-      <c r="CD13" s="13"/>
-      <c r="CJ13" s="13"/>
+      <c r="N13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="S13" s="5"/>
+      <c r="T13" s="5"/>
+      <c r="BI13" s="6"/>
+      <c r="CD13" s="5"/>
+      <c r="CJ13" s="5"/>
     </row>
     <row r="14" spans="1:100" x14ac:dyDescent="0.2">
-      <c r="N14" s="13"/>
-      <c r="S14" s="13"/>
-      <c r="BI14" s="14"/>
+      <c r="N14" s="5"/>
+      <c r="S14" s="5"/>
+      <c r="BI14" s="6"/>
     </row>
     <row r="15" spans="1:100" x14ac:dyDescent="0.2">
-      <c r="N15" s="13"/>
-      <c r="S15" s="13"/>
-      <c r="BI15" s="14"/>
+      <c r="N15" s="5"/>
+      <c r="S15" s="5"/>
+      <c r="BI15" s="6"/>
     </row>
     <row r="16" spans="1:100" x14ac:dyDescent="0.2">
-      <c r="N16" s="13"/>
-      <c r="S16" s="13"/>
-      <c r="BI16" s="14"/>
+      <c r="N16" s="5"/>
+      <c r="S16" s="5"/>
+      <c r="BI16" s="6"/>
     </row>
     <row r="17" spans="14:88" x14ac:dyDescent="0.2">
-      <c r="N17" s="13"/>
-      <c r="S17" s="13"/>
-      <c r="BI17" s="14"/>
-      <c r="CJ17" s="13"/>
+      <c r="N17" s="5"/>
+      <c r="S17" s="5"/>
+      <c r="BI17" s="6"/>
+      <c r="CJ17" s="5"/>
     </row>
     <row r="18" spans="14:88" x14ac:dyDescent="0.2">
-      <c r="N18" s="13"/>
-      <c r="S18" s="13"/>
-      <c r="BI18" s="14"/>
-      <c r="CJ18" s="13"/>
+      <c r="N18" s="5"/>
+      <c r="S18" s="5"/>
+      <c r="BI18" s="6"/>
+      <c r="CJ18" s="5"/>
     </row>
     <row r="19" spans="14:88" x14ac:dyDescent="0.2">
-      <c r="N19" s="13"/>
-      <c r="S19" s="13"/>
-      <c r="BI19" s="14"/>
+      <c r="N19" s="5"/>
+      <c r="S19" s="5"/>
+      <c r="BI19" s="6"/>
     </row>
     <row r="20" spans="14:88" x14ac:dyDescent="0.2">
-      <c r="N20" s="13"/>
-      <c r="Q20" s="13"/>
-      <c r="S20" s="13"/>
-      <c r="BI20" s="14"/>
+      <c r="N20" s="5"/>
+      <c r="Q20" s="5"/>
+      <c r="S20" s="5"/>
+      <c r="BI20" s="6"/>
     </row>
     <row r="21" spans="14:88" x14ac:dyDescent="0.2">
-      <c r="N21" s="13"/>
-      <c r="S21" s="13"/>
-      <c r="BI21" s="14"/>
+      <c r="N21" s="5"/>
+      <c r="S21" s="5"/>
+      <c r="BI21" s="6"/>
     </row>
     <row r="22" spans="14:88" x14ac:dyDescent="0.2">
-      <c r="N22" s="13"/>
-      <c r="O22" s="13"/>
-      <c r="P22" s="13"/>
-      <c r="S22" s="13"/>
-      <c r="BI22" s="14"/>
-      <c r="CD22" s="13"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
+      <c r="S22" s="5"/>
+      <c r="BI22" s="6"/>
+      <c r="CD22" s="5"/>
     </row>
     <row r="23" spans="14:88" x14ac:dyDescent="0.2">
-      <c r="N23" s="13"/>
-      <c r="O23" s="13"/>
-      <c r="P23" s="13"/>
-      <c r="S23" s="13"/>
-      <c r="BI23" s="14"/>
-      <c r="CD23" s="13"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
+      <c r="S23" s="5"/>
+      <c r="BI23" s="6"/>
+      <c r="CD23" s="5"/>
     </row>
     <row r="24" spans="14:88" x14ac:dyDescent="0.2">
-      <c r="N24" s="13"/>
-      <c r="O24" s="13"/>
-      <c r="P24" s="13"/>
-      <c r="S24" s="13"/>
-      <c r="BI24" s="14"/>
-      <c r="CD24" s="13"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
+      <c r="P24" s="5"/>
+      <c r="S24" s="5"/>
+      <c r="BI24" s="6"/>
+      <c r="CD24" s="5"/>
     </row>
     <row r="25" spans="14:88" x14ac:dyDescent="0.2">
-      <c r="N25" s="13"/>
-      <c r="S25" s="13"/>
-      <c r="BI25" s="14"/>
+      <c r="N25" s="5"/>
+      <c r="S25" s="5"/>
+      <c r="BI25" s="6"/>
     </row>
     <row r="26" spans="14:88" x14ac:dyDescent="0.2">
-      <c r="N26" s="13"/>
-      <c r="S26" s="13"/>
-      <c r="BI26" s="14"/>
+      <c r="N26" s="5"/>
+      <c r="S26" s="5"/>
+      <c r="BI26" s="6"/>
     </row>
     <row r="27" spans="14:88" x14ac:dyDescent="0.2">
-      <c r="N27" s="13"/>
-      <c r="S27" s="13"/>
-      <c r="BI27" s="14"/>
-      <c r="CJ27" s="13"/>
+      <c r="N27" s="5"/>
+      <c r="S27" s="5"/>
+      <c r="BI27" s="6"/>
+      <c r="CJ27" s="5"/>
     </row>
     <row r="28" spans="14:88" x14ac:dyDescent="0.2">
-      <c r="N28" s="13"/>
-      <c r="S28" s="13"/>
-      <c r="BI28" s="14"/>
-      <c r="CJ28" s="13"/>
+      <c r="N28" s="5"/>
+      <c r="S28" s="5"/>
+      <c r="BI28" s="6"/>
+      <c r="CJ28" s="5"/>
     </row>
     <row r="29" spans="14:88" x14ac:dyDescent="0.2">
-      <c r="N29" s="13"/>
-      <c r="S29" s="13"/>
-      <c r="BI29" s="14"/>
-      <c r="CJ29" s="13"/>
+      <c r="N29" s="5"/>
+      <c r="S29" s="5"/>
+      <c r="BI29" s="6"/>
+      <c r="CJ29" s="5"/>
     </row>
     <row r="30" spans="14:88" x14ac:dyDescent="0.2">
-      <c r="N30" s="13"/>
-      <c r="O30" s="13"/>
-      <c r="P30" s="13"/>
-      <c r="S30" s="13"/>
-      <c r="BI30" s="14"/>
-      <c r="CD30" s="13"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="5"/>
+      <c r="P30" s="5"/>
+      <c r="S30" s="5"/>
+      <c r="BI30" s="6"/>
+      <c r="CD30" s="5"/>
     </row>
     <row r="31" spans="14:88" x14ac:dyDescent="0.2">
-      <c r="N31" s="13"/>
-      <c r="O31" s="13"/>
-      <c r="P31" s="13"/>
-      <c r="S31" s="13"/>
-      <c r="BI31" s="14"/>
-      <c r="CD31" s="13"/>
-      <c r="CJ31" s="13"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="5"/>
+      <c r="P31" s="5"/>
+      <c r="S31" s="5"/>
+      <c r="BI31" s="6"/>
+      <c r="CD31" s="5"/>
+      <c r="CJ31" s="5"/>
     </row>
     <row r="32" spans="14:88" x14ac:dyDescent="0.2">
-      <c r="N32" s="13"/>
-      <c r="S32" s="13"/>
-      <c r="T32" s="13"/>
-      <c r="BI32" s="14"/>
-      <c r="CD32" s="13"/>
-      <c r="CJ32" s="13"/>
+      <c r="N32" s="5"/>
+      <c r="S32" s="5"/>
+      <c r="T32" s="5"/>
+      <c r="BI32" s="6"/>
+      <c r="CD32" s="5"/>
+      <c r="CJ32" s="5"/>
     </row>
     <row r="33" spans="14:88" x14ac:dyDescent="0.2">
-      <c r="N33" s="13"/>
-      <c r="S33" s="13"/>
-      <c r="T33" s="13"/>
-      <c r="BI33" s="14"/>
-      <c r="CD33" s="13"/>
+      <c r="N33" s="5"/>
+      <c r="S33" s="5"/>
+      <c r="T33" s="5"/>
+      <c r="BI33" s="6"/>
+      <c r="CD33" s="5"/>
     </row>
     <row r="34" spans="14:88" x14ac:dyDescent="0.2">
-      <c r="N34" s="13"/>
-      <c r="S34" s="13"/>
-      <c r="U34" s="13"/>
-      <c r="BI34" s="14"/>
-      <c r="CD34" s="13"/>
+      <c r="N34" s="5"/>
+      <c r="S34" s="5"/>
+      <c r="U34" s="5"/>
+      <c r="BI34" s="6"/>
+      <c r="CD34" s="5"/>
     </row>
     <row r="35" spans="14:88" x14ac:dyDescent="0.2">
-      <c r="N35" s="13"/>
-      <c r="S35" s="13"/>
-      <c r="U35" s="13"/>
-      <c r="BI35" s="14"/>
-      <c r="CD35" s="13"/>
+      <c r="N35" s="5"/>
+      <c r="S35" s="5"/>
+      <c r="U35" s="5"/>
+      <c r="BI35" s="6"/>
+      <c r="CD35" s="5"/>
     </row>
     <row r="36" spans="14:88" x14ac:dyDescent="0.2">
-      <c r="N36" s="13"/>
-      <c r="S36" s="13"/>
-      <c r="U36" s="13"/>
-      <c r="BI36" s="14"/>
-      <c r="CD36" s="13"/>
-      <c r="CJ36" s="13"/>
+      <c r="N36" s="5"/>
+      <c r="S36" s="5"/>
+      <c r="U36" s="5"/>
+      <c r="BI36" s="6"/>
+      <c r="CD36" s="5"/>
+      <c r="CJ36" s="5"/>
     </row>
     <row r="37" spans="14:88" x14ac:dyDescent="0.2">
-      <c r="N37" s="13"/>
-      <c r="S37" s="13"/>
-      <c r="U37" s="13"/>
-      <c r="BI37" s="14"/>
-      <c r="CD37" s="13"/>
-      <c r="CJ37" s="13"/>
+      <c r="N37" s="5"/>
+      <c r="S37" s="5"/>
+      <c r="U37" s="5"/>
+      <c r="BI37" s="6"/>
+      <c r="CD37" s="5"/>
+      <c r="CJ37" s="5"/>
     </row>
     <row r="38" spans="14:88" x14ac:dyDescent="0.2">
-      <c r="N38" s="13"/>
-      <c r="S38" s="13"/>
-      <c r="U38" s="13"/>
-      <c r="BI38" s="14"/>
-      <c r="CD38" s="13"/>
+      <c r="N38" s="5"/>
+      <c r="S38" s="5"/>
+      <c r="U38" s="5"/>
+      <c r="BI38" s="6"/>
+      <c r="CD38" s="5"/>
     </row>
     <row r="39" spans="14:88" x14ac:dyDescent="0.2">
-      <c r="N39" s="13"/>
-      <c r="S39" s="13"/>
-      <c r="U39" s="13"/>
-      <c r="BI39" s="14"/>
-      <c r="CD39" s="13"/>
+      <c r="N39" s="5"/>
+      <c r="S39" s="5"/>
+      <c r="U39" s="5"/>
+      <c r="BI39" s="6"/>
+      <c r="CD39" s="5"/>
     </row>
     <row r="40" spans="14:88" x14ac:dyDescent="0.2">
-      <c r="N40" s="13"/>
-      <c r="Q40" s="13"/>
-      <c r="S40" s="13"/>
-      <c r="U40" s="13"/>
-      <c r="BI40" s="14"/>
-      <c r="CD40" s="13"/>
+      <c r="N40" s="5"/>
+      <c r="Q40" s="5"/>
+      <c r="S40" s="5"/>
+      <c r="U40" s="5"/>
+      <c r="BI40" s="6"/>
+      <c r="CD40" s="5"/>
     </row>
     <row r="41" spans="14:88" x14ac:dyDescent="0.2">
-      <c r="N41" s="13"/>
-      <c r="S41" s="13"/>
-      <c r="U41" s="13"/>
-      <c r="BI41" s="14"/>
-      <c r="CD41" s="13"/>
+      <c r="N41" s="5"/>
+      <c r="S41" s="5"/>
+      <c r="U41" s="5"/>
+      <c r="BI41" s="6"/>
+      <c r="CD41" s="5"/>
     </row>
     <row r="42" spans="14:88" x14ac:dyDescent="0.2">
-      <c r="N42" s="13"/>
-      <c r="S42" s="13"/>
-      <c r="U42" s="13"/>
-      <c r="BI42" s="14"/>
-      <c r="CD42" s="13"/>
+      <c r="N42" s="5"/>
+      <c r="S42" s="5"/>
+      <c r="U42" s="5"/>
+      <c r="BI42" s="6"/>
+      <c r="CD42" s="5"/>
     </row>
     <row r="43" spans="14:88" x14ac:dyDescent="0.2">
-      <c r="N43" s="13"/>
-      <c r="S43" s="13"/>
-      <c r="U43" s="13"/>
-      <c r="BI43" s="14"/>
-      <c r="CD43" s="13"/>
-      <c r="CJ43" s="13"/>
+      <c r="N43" s="5"/>
+      <c r="S43" s="5"/>
+      <c r="U43" s="5"/>
+      <c r="BI43" s="6"/>
+      <c r="CD43" s="5"/>
+      <c r="CJ43" s="5"/>
     </row>
     <row r="44" spans="14:88" x14ac:dyDescent="0.2">
-      <c r="N44" s="13"/>
-      <c r="S44" s="13"/>
-      <c r="U44" s="13"/>
-      <c r="BI44" s="14"/>
-      <c r="CD44" s="13"/>
+      <c r="N44" s="5"/>
+      <c r="S44" s="5"/>
+      <c r="U44" s="5"/>
+      <c r="BI44" s="6"/>
+      <c r="CD44" s="5"/>
     </row>
     <row r="45" spans="14:88" x14ac:dyDescent="0.2">
-      <c r="N45" s="13"/>
-      <c r="S45" s="13"/>
-      <c r="U45" s="13"/>
-      <c r="BI45" s="14"/>
-      <c r="CD45" s="13"/>
+      <c r="N45" s="5"/>
+      <c r="S45" s="5"/>
+      <c r="U45" s="5"/>
+      <c r="BI45" s="6"/>
+      <c r="CD45" s="5"/>
     </row>
     <row r="46" spans="14:88" x14ac:dyDescent="0.2">
-      <c r="N46" s="13"/>
-      <c r="O46" s="13"/>
-      <c r="P46" s="13"/>
-      <c r="S46" s="13"/>
-      <c r="BI46" s="14"/>
-      <c r="CD46" s="13"/>
+      <c r="N46" s="5"/>
+      <c r="O46" s="5"/>
+      <c r="P46" s="5"/>
+      <c r="S46" s="5"/>
+      <c r="BI46" s="6"/>
+      <c r="CD46" s="5"/>
     </row>
     <row r="47" spans="14:88" x14ac:dyDescent="0.2">
-      <c r="N47" s="13"/>
-      <c r="O47" s="13"/>
-      <c r="P47" s="13"/>
-      <c r="S47" s="13"/>
-      <c r="BI47" s="14"/>
-      <c r="CD47" s="13"/>
-      <c r="CJ47" s="13"/>
+      <c r="N47" s="5"/>
+      <c r="O47" s="5"/>
+      <c r="P47" s="5"/>
+      <c r="S47" s="5"/>
+      <c r="BI47" s="6"/>
+      <c r="CD47" s="5"/>
+      <c r="CJ47" s="5"/>
     </row>
     <row r="48" spans="14:88" x14ac:dyDescent="0.2">
-      <c r="N48" s="13"/>
-      <c r="O48" s="13"/>
-      <c r="P48" s="13"/>
-      <c r="S48" s="13"/>
-      <c r="BI48" s="14"/>
-      <c r="CD48" s="13"/>
+      <c r="N48" s="5"/>
+      <c r="O48" s="5"/>
+      <c r="P48" s="5"/>
+      <c r="S48" s="5"/>
+      <c r="BI48" s="6"/>
+      <c r="CD48" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2485,8 +2424,321 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4431688-BB01-D444-AD6D-CA9792BD8EF3}">
+  <dimension ref="A1:CV1"/>
+  <sheetViews>
+    <sheetView topLeftCell="BO1" workbookViewId="0">
+      <selection activeCell="BZ1" sqref="A1:CT1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:100" ht="76" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>385</v>
+      </c>
+      <c r="B1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C1" t="s">
+        <v>287</v>
+      </c>
+      <c r="D1" t="s">
+        <v>288</v>
+      </c>
+      <c r="E1" t="s">
+        <v>289</v>
+      </c>
+      <c r="F1" t="s">
+        <v>290</v>
+      </c>
+      <c r="G1" t="s">
+        <v>291</v>
+      </c>
+      <c r="H1" t="s">
+        <v>292</v>
+      </c>
+      <c r="I1" t="s">
+        <v>293</v>
+      </c>
+      <c r="J1" t="s">
+        <v>294</v>
+      </c>
+      <c r="K1" t="s">
+        <v>295</v>
+      </c>
+      <c r="L1" t="s">
+        <v>296</v>
+      </c>
+      <c r="M1" t="s">
+        <v>297</v>
+      </c>
+      <c r="N1" t="s">
+        <v>298</v>
+      </c>
+      <c r="O1" t="s">
+        <v>415</v>
+      </c>
+      <c r="P1" t="s">
+        <v>416</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>301</v>
+      </c>
+      <c r="R1" t="s">
+        <v>302</v>
+      </c>
+      <c r="S1" t="s">
+        <v>303</v>
+      </c>
+      <c r="T1" t="s">
+        <v>304</v>
+      </c>
+      <c r="U1" t="s">
+        <v>305</v>
+      </c>
+      <c r="V1" t="s">
+        <v>417</v>
+      </c>
+      <c r="W1" t="s">
+        <v>307</v>
+      </c>
+      <c r="X1" t="s">
+        <v>418</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>309</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>419</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>420</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>311</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>312</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>313</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>314</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>315</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>316</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>317</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>318</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>319</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>320</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>321</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>322</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>323</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>324</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>325</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>326</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>421</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>422</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>327</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>328</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>329</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>330</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>331</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>332</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>333</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>336</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>337</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>338</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>340</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>423</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>343</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>344</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>345</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>346</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>347</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>424</v>
+      </c>
+      <c r="BL1" t="s">
+        <v>348</v>
+      </c>
+      <c r="BM1" t="s">
+        <v>350</v>
+      </c>
+      <c r="BN1" t="s">
+        <v>352</v>
+      </c>
+      <c r="BO1" t="s">
+        <v>353</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>354</v>
+      </c>
+      <c r="BQ1" t="s">
+        <v>355</v>
+      </c>
+      <c r="BR1" t="s">
+        <v>356</v>
+      </c>
+      <c r="BS1" t="s">
+        <v>357</v>
+      </c>
+      <c r="BT1" t="s">
+        <v>358</v>
+      </c>
+      <c r="BU1" t="s">
+        <v>359</v>
+      </c>
+      <c r="BV1" t="s">
+        <v>361</v>
+      </c>
+      <c r="BW1" t="s">
+        <v>362</v>
+      </c>
+      <c r="BX1" t="s">
+        <v>363</v>
+      </c>
+      <c r="BY1" t="s">
+        <v>364</v>
+      </c>
+      <c r="BZ1" t="s">
+        <v>365</v>
+      </c>
+      <c r="CA1" t="s">
+        <v>425</v>
+      </c>
+      <c r="CB1" t="s">
+        <v>426</v>
+      </c>
+      <c r="CC1" t="s">
+        <v>366</v>
+      </c>
+      <c r="CD1" t="s">
+        <v>367</v>
+      </c>
+      <c r="CE1" t="s">
+        <v>368</v>
+      </c>
+      <c r="CF1" t="s">
+        <v>369</v>
+      </c>
+      <c r="CG1" t="s">
+        <v>370</v>
+      </c>
+      <c r="CH1" t="s">
+        <v>371</v>
+      </c>
+      <c r="CI1" t="s">
+        <v>372</v>
+      </c>
+      <c r="CJ1" t="s">
+        <v>373</v>
+      </c>
+      <c r="CK1" t="s">
+        <v>374</v>
+      </c>
+      <c r="CL1" t="s">
+        <v>375</v>
+      </c>
+      <c r="CM1" t="s">
+        <v>377</v>
+      </c>
+      <c r="CN1" t="s">
+        <v>378</v>
+      </c>
+      <c r="CO1" t="s">
+        <v>380</v>
+      </c>
+      <c r="CP1" t="s">
+        <v>427</v>
+      </c>
+      <c r="CQ1" t="s">
+        <v>381</v>
+      </c>
+      <c r="CR1" t="s">
+        <v>382</v>
+      </c>
+      <c r="CS1" t="s">
+        <v>383</v>
+      </c>
+      <c r="CT1" t="s">
+        <v>384</v>
+      </c>
+      <c r="CU1" s="9"/>
+      <c r="CV1" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39D62796-E255-9B43-871F-22ACFD2C6852}">
-  <dimension ref="A1:KA3"/>
+  <dimension ref="A1:KC3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -2494,905 +2746,910 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.5" style="11" customWidth="1"/>
-    <col min="2" max="287" width="21.6640625" style="11" customWidth="1"/>
-    <col min="288" max="16384" width="8.83203125" style="11"/>
+    <col min="1" max="1" width="19.83203125" style="3" customWidth="1"/>
+    <col min="2" max="3" width="33.5" style="3" customWidth="1"/>
+    <col min="4" max="289" width="21.6640625" style="3" customWidth="1"/>
+    <col min="290" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:287" ht="48" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
-        <v>417</v>
-      </c>
-      <c r="B1" s="10" t="s">
+    <row r="1" spans="1:289" ht="48" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>399</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>414</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="AK1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="AL1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="AM1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="AN1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="AO1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="AP1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="AR1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="AS1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="AT1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="AU1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="AV1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="AW1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="Q1" s="10" t="s">
+      <c r="AX1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="AY1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="BA1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="U1" s="10" t="s">
+      <c r="BB1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="V1" s="10" t="s">
+      <c r="BC1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="W1" s="10" t="s">
+      <c r="BD1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="X1" s="10" t="s">
+      <c r="BE1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="Y1" s="10" t="s">
+      <c r="BF1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="Z1" s="10" t="s">
+      <c r="BG1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="AA1" s="10" t="s">
+      <c r="BH1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="AB1" s="10" t="s">
+      <c r="BI1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="AC1" s="10" t="s">
+      <c r="BJ1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="AD1" s="10" t="s">
+      <c r="BK1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="AE1" s="10" t="s">
+      <c r="BL1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="AF1" s="10" t="s">
+      <c r="BM1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="AG1" s="10" t="s">
+      <c r="BN1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="AH1" s="10" t="s">
+      <c r="BO1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="AI1" s="10" t="s">
+      <c r="BP1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="AJ1" s="10" t="s">
+      <c r="BQ1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="AK1" s="10" t="s">
+      <c r="BR1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="AL1" s="10" t="s">
+      <c r="BS1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="AM1" s="10" t="s">
+      <c r="BT1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="AN1" s="10" t="s">
+      <c r="BU1" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="AO1" s="10" t="s">
+      <c r="BV1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="AP1" s="10" t="s">
+      <c r="BW1" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="AQ1" s="10" t="s">
+      <c r="BX1" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="AR1" s="10" t="s">
+      <c r="BY1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="AS1" s="10" t="s">
+      <c r="BZ1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AT1" s="10" t="s">
+      <c r="CA1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="AU1" s="10" t="s">
+      <c r="CB1" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="AV1" s="10" t="s">
+      <c r="CC1" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AW1" s="10" t="s">
+      <c r="CD1" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="AX1" s="10" t="s">
+      <c r="CE1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="AY1" s="10" t="s">
+      <c r="CF1" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="AZ1" s="10" t="s">
+      <c r="CG1" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="BA1" s="10" t="s">
+      <c r="CH1" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="BB1" s="10" t="s">
+      <c r="CI1" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="BC1" s="10" t="s">
+      <c r="CJ1" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="BD1" s="10" t="s">
+      <c r="CK1" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="BE1" s="10" t="s">
+      <c r="CL1" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="BF1" s="10" t="s">
+      <c r="CM1" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="BG1" s="10" t="s">
+      <c r="CN1" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="BH1" s="10" t="s">
+      <c r="CO1" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="BI1" s="10" t="s">
+      <c r="CP1" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="BJ1" s="10" t="s">
+      <c r="CQ1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="BK1" s="10" t="s">
+      <c r="CR1" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="BL1" s="10" t="s">
+      <c r="CS1" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="BM1" s="10" t="s">
+      <c r="CT1" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="BN1" s="10" t="s">
+      <c r="CU1" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="BO1" s="10" t="s">
+      <c r="CV1" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="BP1" s="10" t="s">
+      <c r="CW1" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="BQ1" s="10" t="s">
+      <c r="CX1" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="BR1" s="10" t="s">
+      <c r="CY1" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="BS1" s="10" t="s">
+      <c r="CZ1" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="BT1" s="10" t="s">
+      <c r="DA1" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="BU1" s="10" t="s">
+      <c r="DB1" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="BV1" s="10" t="s">
+      <c r="DC1" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="BW1" s="10" t="s">
+      <c r="DD1" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="BX1" s="10" t="s">
+      <c r="DE1" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="BY1" s="10" t="s">
+      <c r="DF1" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="BZ1" s="10" t="s">
+      <c r="DG1" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="CA1" s="10" t="s">
+      <c r="DH1" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="CB1" s="10" t="s">
+      <c r="DI1" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="CC1" s="10" t="s">
+      <c r="DJ1" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="CD1" s="10" t="s">
+      <c r="DK1" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="CE1" s="10" t="s">
+      <c r="DL1" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="CF1" s="10" t="s">
+      <c r="DM1" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="CG1" s="10" t="s">
+      <c r="DN1" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="CH1" s="10" t="s">
+      <c r="DO1" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="CI1" s="10" t="s">
+      <c r="DP1" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="CJ1" s="10" t="s">
+      <c r="DQ1" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="CK1" s="10" t="s">
+      <c r="DR1" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="CL1" s="10" t="s">
+      <c r="DS1" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="CM1" s="10" t="s">
+      <c r="DT1" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="CN1" s="10" t="s">
+      <c r="DU1" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="CO1" s="10" t="s">
+      <c r="DV1" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="CP1" s="10" t="s">
+      <c r="DW1" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="CQ1" s="10" t="s">
+      <c r="DX1" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="CR1" s="10" t="s">
+      <c r="DY1" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="CS1" s="10" t="s">
+      <c r="DZ1" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="CT1" s="10" t="s">
+      <c r="EA1" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="CU1" s="10" t="s">
+      <c r="EB1" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="CV1" s="10" t="s">
+      <c r="EC1" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="CW1" s="10" t="s">
+      <c r="ED1" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="CX1" s="10" t="s">
+      <c r="EE1" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="CY1" s="10" t="s">
+      <c r="EF1" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="CZ1" s="10" t="s">
+      <c r="EG1" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="DA1" s="10" t="s">
+      <c r="EH1" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="DB1" s="10" t="s">
+      <c r="EI1" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="DC1" s="10" t="s">
+      <c r="EJ1" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="DD1" s="10" t="s">
+      <c r="EK1" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="DE1" s="10" t="s">
+      <c r="EL1" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="DF1" s="10" t="s">
+      <c r="EM1" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="DG1" s="10" t="s">
+      <c r="EN1" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="DH1" s="10" t="s">
+      <c r="EO1" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="DI1" s="10" t="s">
+      <c r="EP1" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="DJ1" s="10" t="s">
+      <c r="EQ1" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="DK1" s="10" t="s">
+      <c r="ER1" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="DL1" s="10" t="s">
+      <c r="ES1" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="DM1" s="10" t="s">
+      <c r="ET1" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="DN1" s="10" t="s">
+      <c r="EU1" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="DO1" s="10" t="s">
+      <c r="EV1" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="DP1" s="10" t="s">
+      <c r="EW1" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="DQ1" s="10" t="s">
+      <c r="EX1" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="DR1" s="10" t="s">
+      <c r="EY1" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="DS1" s="10" t="s">
+      <c r="EZ1" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="DT1" s="10" t="s">
+      <c r="FA1" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="DU1" s="10" t="s">
+      <c r="FB1" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="DV1" s="10" t="s">
+      <c r="FC1" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="DW1" s="10" t="s">
+      <c r="FD1" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="DX1" s="10" t="s">
+      <c r="FE1" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="DY1" s="10" t="s">
+      <c r="FF1" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="DZ1" s="10" t="s">
+      <c r="FG1" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="EA1" s="10" t="s">
+      <c r="FH1" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="EB1" s="10" t="s">
+      <c r="FI1" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="EC1" s="10" t="s">
+      <c r="FJ1" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="ED1" s="10" t="s">
+      <c r="FK1" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="EE1" s="10" t="s">
+      <c r="FL1" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="EF1" s="10" t="s">
+      <c r="FM1" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="EG1" s="10" t="s">
+      <c r="FN1" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="EH1" s="10" t="s">
+      <c r="FO1" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="EI1" s="10" t="s">
+      <c r="FP1" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="EJ1" s="10" t="s">
+      <c r="FQ1" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="EK1" s="10" t="s">
+      <c r="FR1" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="EL1" s="10" t="s">
+      <c r="FS1" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="EM1" s="10" t="s">
+      <c r="FT1" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="EN1" s="10" t="s">
+      <c r="FU1" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="EO1" s="10" t="s">
+      <c r="FV1" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="EP1" s="10" t="s">
+      <c r="FW1" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="EQ1" s="10" t="s">
+      <c r="FX1" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="ER1" s="10" t="s">
+      <c r="FY1" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="ES1" s="10" t="s">
+      <c r="FZ1" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="ET1" s="10" t="s">
+      <c r="GA1" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="EU1" s="10" t="s">
+      <c r="GB1" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="EV1" s="10" t="s">
+      <c r="GC1" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="EW1" s="10" t="s">
+      <c r="GD1" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="EX1" s="10" t="s">
+      <c r="GE1" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="EY1" s="10" t="s">
+      <c r="GF1" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="EZ1" s="10" t="s">
+      <c r="GG1" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="FA1" s="10" t="s">
+      <c r="GH1" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="FB1" s="10" t="s">
+      <c r="GI1" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="FC1" s="10" t="s">
+      <c r="GJ1" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="FD1" s="10" t="s">
+      <c r="GK1" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="FE1" s="10" t="s">
+      <c r="GL1" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="FF1" s="10" t="s">
+      <c r="GM1" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="FG1" s="10" t="s">
+      <c r="GN1" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="FH1" s="10" t="s">
+      <c r="GO1" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="FI1" s="10" t="s">
+      <c r="GP1" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="FJ1" s="10" t="s">
+      <c r="GQ1" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="FK1" s="10" t="s">
+      <c r="GR1" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="FL1" s="10" t="s">
+      <c r="GS1" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="FM1" s="10" t="s">
+      <c r="GT1" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="FN1" s="10" t="s">
+      <c r="GU1" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="FO1" s="10" t="s">
+      <c r="GV1" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="FP1" s="10" t="s">
+      <c r="GW1" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="FQ1" s="10" t="s">
+      <c r="GX1" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="FR1" s="10" t="s">
+      <c r="GY1" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="FS1" s="10" t="s">
+      <c r="GZ1" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="FT1" s="10" t="s">
+      <c r="HA1" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="FU1" s="10" t="s">
+      <c r="HB1" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="FV1" s="10" t="s">
+      <c r="HC1" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="FW1" s="10" t="s">
+      <c r="HD1" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="FX1" s="10" t="s">
+      <c r="HE1" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="FY1" s="10" t="s">
+      <c r="HF1" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="FZ1" s="10" t="s">
+      <c r="HG1" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="GA1" s="10" t="s">
+      <c r="HH1" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="GB1" s="10" t="s">
+      <c r="HI1" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="GC1" s="10" t="s">
+      <c r="HJ1" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="GD1" s="10" t="s">
+      <c r="HK1" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="GE1" s="10" t="s">
+      <c r="HL1" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="GF1" s="10" t="s">
+      <c r="HM1" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="GG1" s="10" t="s">
+      <c r="HN1" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="GH1" s="10" t="s">
+      <c r="HO1" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="GI1" s="10" t="s">
+      <c r="HP1" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="GJ1" s="10" t="s">
+      <c r="HQ1" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="GK1" s="10" t="s">
+      <c r="HR1" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="GL1" s="10" t="s">
+      <c r="HS1" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="GM1" s="10" t="s">
+      <c r="HT1" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="GN1" s="10" t="s">
+      <c r="HU1" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="GO1" s="10" t="s">
+      <c r="HV1" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="GP1" s="10" t="s">
+      <c r="HW1" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="GQ1" s="10" t="s">
+      <c r="HX1" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="GR1" s="10" t="s">
+      <c r="HY1" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="GS1" s="10" t="s">
+      <c r="HZ1" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="GT1" s="10" t="s">
+      <c r="IA1" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="GU1" s="10" t="s">
+      <c r="IB1" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="GV1" s="10" t="s">
+      <c r="IC1" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="GW1" s="10" t="s">
+      <c r="ID1" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="GX1" s="10" t="s">
+      <c r="IE1" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="GY1" s="10" t="s">
+      <c r="IF1" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="GZ1" s="10" t="s">
+      <c r="IG1" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="HA1" s="10" t="s">
+      <c r="IH1" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="HB1" s="10" t="s">
+      <c r="II1" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="HC1" s="10" t="s">
+      <c r="IJ1" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="HD1" s="10" t="s">
+      <c r="IK1" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="HE1" s="10" t="s">
+      <c r="IL1" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="HF1" s="10" t="s">
+      <c r="IM1" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="HG1" s="10" t="s">
+      <c r="IN1" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="HH1" s="10" t="s">
+      <c r="IO1" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="HI1" s="10" t="s">
+      <c r="IP1" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="HJ1" s="10" t="s">
+      <c r="IQ1" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="HK1" s="10" t="s">
+      <c r="IR1" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="HL1" s="10" t="s">
+      <c r="IS1" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="HM1" s="10" t="s">
+      <c r="IT1" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="HN1" s="10" t="s">
+      <c r="IU1" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="HO1" s="10" t="s">
+      <c r="IV1" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="HP1" s="10" t="s">
+      <c r="IW1" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="HQ1" s="10" t="s">
+      <c r="IX1" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="HR1" s="10" t="s">
+      <c r="IY1" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="HS1" s="10" t="s">
+      <c r="IZ1" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="HT1" s="10" t="s">
+      <c r="JA1" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="HU1" s="10" t="s">
+      <c r="JB1" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="HV1" s="10" t="s">
+      <c r="JC1" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="HW1" s="10" t="s">
+      <c r="JD1" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="HX1" s="10" t="s">
+      <c r="JE1" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="HY1" s="10" t="s">
+      <c r="JF1" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="HZ1" s="10" t="s">
+      <c r="JG1" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="IA1" s="10" t="s">
+      <c r="JH1" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="IB1" s="10" t="s">
+      <c r="JI1" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="IC1" s="10" t="s">
+      <c r="JJ1" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="ID1" s="10" t="s">
+      <c r="JK1" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="IE1" s="10" t="s">
+      <c r="JL1" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="IF1" s="10" t="s">
+      <c r="JM1" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="IG1" s="10" t="s">
+      <c r="JN1" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="IH1" s="10" t="s">
+      <c r="JO1" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="II1" s="10" t="s">
+      <c r="JP1" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="IJ1" s="10" t="s">
+      <c r="JQ1" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="IK1" s="10" t="s">
+      <c r="JR1" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="IL1" s="10" t="s">
+      <c r="JS1" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="IM1" s="10" t="s">
+      <c r="JT1" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="IN1" s="10" t="s">
+      <c r="JU1" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="IO1" s="10" t="s">
+      <c r="JV1" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="IP1" s="10" t="s">
+      <c r="JW1" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="IQ1" s="10" t="s">
+      <c r="JX1" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="IR1" s="10" t="s">
+      <c r="JY1" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="IS1" s="10" t="s">
+      <c r="JZ1" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="IT1" s="10" t="s">
+      <c r="KA1" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="IU1" s="10" t="s">
+      <c r="KB1" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="IV1" s="10" t="s">
-        <v>286</v>
-      </c>
-      <c r="IW1" s="10" t="s">
-        <v>287</v>
-      </c>
-      <c r="IX1" s="10" t="s">
-        <v>288</v>
-      </c>
-      <c r="IY1" s="10" t="s">
-        <v>289</v>
-      </c>
-      <c r="IZ1" s="10" t="s">
-        <v>290</v>
-      </c>
-      <c r="JA1" s="10" t="s">
-        <v>291</v>
-      </c>
-      <c r="JB1" s="10" t="s">
-        <v>292</v>
-      </c>
-      <c r="JC1" s="10" t="s">
-        <v>293</v>
-      </c>
-      <c r="JD1" s="10" t="s">
-        <v>294</v>
-      </c>
-      <c r="JE1" s="10" t="s">
-        <v>295</v>
-      </c>
-      <c r="JF1" s="10" t="s">
-        <v>296</v>
-      </c>
-      <c r="JG1" s="10" t="s">
-        <v>297</v>
-      </c>
-      <c r="JH1" s="10" t="s">
-        <v>298</v>
-      </c>
-      <c r="JI1" s="10" t="s">
-        <v>299</v>
-      </c>
-      <c r="JJ1" s="10" t="s">
-        <v>300</v>
-      </c>
-      <c r="JK1" s="10" t="s">
-        <v>301</v>
-      </c>
-      <c r="JL1" s="10" t="s">
-        <v>302</v>
-      </c>
-      <c r="JM1" s="10" t="s">
-        <v>303</v>
-      </c>
-      <c r="JN1" s="10" t="s">
-        <v>304</v>
-      </c>
-      <c r="JO1" s="10" t="s">
-        <v>305</v>
-      </c>
-      <c r="JP1" s="10" t="s">
-        <v>306</v>
-      </c>
-      <c r="JQ1" s="10" t="s">
-        <v>307</v>
-      </c>
-      <c r="JR1" s="10" t="s">
-        <v>308</v>
-      </c>
-      <c r="JS1" s="10" t="s">
-        <v>309</v>
-      </c>
-      <c r="JT1" s="10" t="s">
-        <v>310</v>
-      </c>
-      <c r="JU1" s="10" t="s">
-        <v>311</v>
-      </c>
-      <c r="JV1" s="10" t="s">
-        <v>312</v>
-      </c>
-      <c r="JW1" s="10" t="s">
-        <v>313</v>
-      </c>
-      <c r="JX1" s="10" t="s">
-        <v>314</v>
-      </c>
-      <c r="JY1" s="10" t="s">
-        <v>315</v>
-      </c>
-      <c r="JZ1" s="10" t="s">
-        <v>316</v>
-      </c>
-      <c r="KA1" s="10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:287" x14ac:dyDescent="0.2">
-      <c r="BI2" s="12"/>
-      <c r="BJ2" s="12"/>
-      <c r="BK2" s="12"/>
-      <c r="HL2" s="12"/>
-      <c r="HO2" s="12"/>
-      <c r="HR2" s="12"/>
-      <c r="HU2" s="12"/>
-      <c r="HX2" s="12"/>
-      <c r="IA2" s="12"/>
-      <c r="ID2" s="12"/>
-      <c r="IG2" s="12"/>
-      <c r="IJ2" s="12"/>
-      <c r="IM2" s="12"/>
-      <c r="IP2" s="12"/>
-      <c r="IS2" s="12"/>
-      <c r="IV2" s="12"/>
-      <c r="IY2" s="12"/>
-      <c r="JB2" s="12"/>
-      <c r="JE2" s="12"/>
-      <c r="JH2" s="12"/>
-      <c r="JK2" s="12"/>
-      <c r="JN2" s="12"/>
-      <c r="JQ2" s="12"/>
-      <c r="JT2" s="12"/>
-      <c r="JW2" s="12"/>
-      <c r="JZ2" s="12"/>
-    </row>
-    <row r="3" spans="1:287" ht="16" x14ac:dyDescent="0.2">
-      <c r="B3"/>
-      <c r="C3"/>
+      <c r="KC1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:289" x14ac:dyDescent="0.2">
+      <c r="BK2" s="4"/>
+      <c r="BL2" s="4"/>
+      <c r="BM2" s="4"/>
+      <c r="HN2" s="4"/>
+      <c r="HQ2" s="4"/>
+      <c r="HT2" s="4"/>
+      <c r="HW2" s="4"/>
+      <c r="HZ2" s="4"/>
+      <c r="IC2" s="4"/>
+      <c r="IF2" s="4"/>
+      <c r="II2" s="4"/>
+      <c r="IL2" s="4"/>
+      <c r="IO2" s="4"/>
+      <c r="IR2" s="4"/>
+      <c r="IU2" s="4"/>
+      <c r="IX2" s="4"/>
+      <c r="JA2" s="4"/>
+      <c r="JD2" s="4"/>
+      <c r="JG2" s="4"/>
+      <c r="JJ2" s="4"/>
+      <c r="JM2" s="4"/>
+      <c r="JP2" s="4"/>
+      <c r="JS2" s="4"/>
+      <c r="JV2" s="4"/>
+      <c r="JY2" s="4"/>
+      <c r="KB2" s="4"/>
+    </row>
+    <row r="3" spans="1:289" ht="16" x14ac:dyDescent="0.2">
       <c r="D3"/>
       <c r="E3"/>
       <c r="F3"/>
@@ -3450,11 +3707,11 @@
       <c r="BF3"/>
       <c r="BG3"/>
       <c r="BH3"/>
-      <c r="BI3" s="12"/>
-      <c r="BJ3" s="12"/>
-      <c r="BK3" s="12"/>
-      <c r="BL3"/>
-      <c r="BM3"/>
+      <c r="BI3"/>
+      <c r="BJ3"/>
+      <c r="BK3" s="4"/>
+      <c r="BL3" s="4"/>
+      <c r="BM3" s="4"/>
       <c r="BN3"/>
       <c r="BO3"/>
       <c r="BP3"/>
@@ -3609,343 +3866,210 @@
       <c r="HI3"/>
       <c r="HJ3"/>
       <c r="HK3"/>
-      <c r="HL3" s="12"/>
+      <c r="HL3"/>
       <c r="HM3"/>
-      <c r="HN3"/>
-      <c r="HO3" s="12"/>
+      <c r="HN3" s="4"/>
+      <c r="HO3"/>
       <c r="HP3"/>
-      <c r="HQ3"/>
-      <c r="HR3" s="12"/>
+      <c r="HQ3" s="4"/>
+      <c r="HR3"/>
       <c r="HS3"/>
-      <c r="HT3"/>
-      <c r="HU3" s="12"/>
+      <c r="HT3" s="4"/>
+      <c r="HU3"/>
       <c r="HV3"/>
-      <c r="HW3"/>
-      <c r="HX3" s="12"/>
+      <c r="HW3" s="4"/>
+      <c r="HX3"/>
       <c r="HY3"/>
-      <c r="HZ3"/>
-      <c r="IA3" s="12"/>
+      <c r="HZ3" s="4"/>
+      <c r="IA3"/>
       <c r="IB3"/>
-      <c r="IC3"/>
-      <c r="ID3" s="12"/>
+      <c r="IC3" s="4"/>
+      <c r="ID3"/>
       <c r="IE3"/>
-      <c r="IF3"/>
-      <c r="IG3" s="12"/>
+      <c r="IF3" s="4"/>
+      <c r="IG3"/>
       <c r="IH3"/>
-      <c r="II3"/>
-      <c r="IJ3" s="12"/>
+      <c r="II3" s="4"/>
+      <c r="IJ3"/>
       <c r="IK3"/>
-      <c r="IL3"/>
-      <c r="IM3" s="12"/>
+      <c r="IL3" s="4"/>
+      <c r="IM3"/>
       <c r="IN3"/>
-      <c r="IO3"/>
-      <c r="IP3" s="12"/>
+      <c r="IO3" s="4"/>
+      <c r="IP3"/>
       <c r="IQ3"/>
-      <c r="IR3"/>
-      <c r="IS3" s="12"/>
+      <c r="IR3" s="4"/>
+      <c r="IS3"/>
       <c r="IT3"/>
-      <c r="IU3"/>
-      <c r="IV3" s="12"/>
+      <c r="IU3" s="4"/>
+      <c r="IV3"/>
       <c r="IW3"/>
-      <c r="IX3"/>
-      <c r="IY3" s="12"/>
+      <c r="IX3" s="4"/>
+      <c r="IY3"/>
       <c r="IZ3"/>
-      <c r="JA3"/>
-      <c r="JB3" s="12"/>
+      <c r="JA3" s="4"/>
+      <c r="JB3"/>
       <c r="JC3"/>
-      <c r="JD3"/>
-      <c r="JE3" s="12"/>
+      <c r="JD3" s="4"/>
+      <c r="JE3"/>
       <c r="JF3"/>
-      <c r="JG3"/>
-      <c r="JH3" s="12"/>
+      <c r="JG3" s="4"/>
+      <c r="JH3"/>
       <c r="JI3"/>
-      <c r="JJ3"/>
-      <c r="JK3" s="12"/>
+      <c r="JJ3" s="4"/>
+      <c r="JK3"/>
       <c r="JL3"/>
-      <c r="JM3"/>
-      <c r="JN3" s="12"/>
+      <c r="JM3" s="4"/>
+      <c r="JN3"/>
       <c r="JO3"/>
-      <c r="JP3"/>
-      <c r="JQ3" s="12"/>
+      <c r="JP3" s="4"/>
+      <c r="JQ3"/>
       <c r="JR3"/>
-      <c r="JS3"/>
-      <c r="JT3" s="12"/>
+      <c r="JS3" s="4"/>
+      <c r="JT3"/>
       <c r="JU3"/>
-      <c r="JV3"/>
-      <c r="JW3" s="12"/>
+      <c r="JV3" s="4"/>
+      <c r="JW3"/>
       <c r="JX3"/>
-      <c r="JY3"/>
-      <c r="JZ3" s="12"/>
+      <c r="JY3" s="4"/>
+      <c r="JZ3"/>
       <c r="KA3"/>
+      <c r="KB3" s="4"/>
+      <c r="KC3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FBF50E7-30AA-B04E-A164-A69234A3E4F0}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:AO1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C56F768-0E6E-1348-9379-5C1FA25B8AC5}">
-  <dimension ref="B3:C6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="83" workbookViewId="0">
+      <selection activeCell="AP1" sqref="AD1:AP1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.5" customWidth="1"/>
-    <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="12.1640625" customWidth="1"/>
+    <col min="15" max="15" width="32" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11" customWidth="1"/>
+    <col min="18" max="18" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="9"/>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>31</v>
-      </c>
+    <row r="1" spans="1:41" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="R1" s="10" t="s">
+        <v>401</v>
+      </c>
+      <c r="S1" s="11" t="s">
+        <v>413</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="AD1" s="12"/>
+      <c r="AE1" s="12"/>
+      <c r="AF1" s="12"/>
+      <c r="AG1" s="12"/>
+      <c r="AH1" s="12"/>
+      <c r="AI1" s="12"/>
+      <c r="AJ1" s="12"/>
+      <c r="AK1" s="12"/>
+      <c r="AL1" s="12"/>
+      <c r="AM1" s="12"/>
+      <c r="AN1" s="12"/>
+      <c r="AO1" s="12"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E237C06-4F78-DB46-A004-0627BBD9559D}">
-  <dimension ref="B2:D29"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="3.33203125" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B2" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="2"/>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B4" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B5" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="5"/>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B6" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="5"/>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="5"/>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="5"/>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="6"/>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="5"/>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="5"/>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B12" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="5"/>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="5"/>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B15" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="5"/>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="5"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B17" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="5"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B18" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="6"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B19" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="5"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B20" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" s="5"/>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B21" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" s="5"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B22" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="5"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B23" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" s="5"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B24" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24" s="5"/>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B25" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B26" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B27" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B28" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B29" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54E05C14-D86D-A249-B13A-6A6C014D3B78}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{524F063A-131C-A54C-A138-24C1EFD46DAE}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="16384" width="10.83203125" style="8"/>
-  </cols>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>